<commit_message>
cleaning up more and more
</commit_message>
<xml_diff>
--- a/figures/figure_xlsx/figures-Dan.xlsx
+++ b/figures/figure_xlsx/figures-Dan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="80" windowWidth="27800" windowHeight="11080" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="80" windowWidth="27800" windowHeight="11080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>translation suggestion</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>undo</t>
-  </si>
-  <si>
-    <t>text to speech</t>
   </si>
   <si>
     <t>alternatives</t>
@@ -177,7 +174,7 @@
                   <c:v>undo</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>text to speech</c:v>
+                  <c:v>pronounciation</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>alternatives</c:v>
@@ -253,6 +250,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -290,6 +288,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -388,7 +387,7 @@
                   <c:v>undo</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>text to speech</c:v>
+                  <c:v>pronounciation</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>alternatives</c:v>
@@ -493,6 +492,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4473,8 +4473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>296</v>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>1146</v>
@@ -4525,7 +4525,7 @@
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>6721</v>
@@ -8539,8 +8539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8575,7 +8575,7 @@
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>45</v>
@@ -8583,7 +8583,7 @@
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
         <v>45</v>
@@ -8591,7 +8591,7 @@
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>57</v>

</xml_diff>